<commit_message>
up new version code
</commit_message>
<xml_diff>
--- a/RFvalue.xlsx
+++ b/RFvalue.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDBASKETBALL\OneDrive\Máy tính\code\HuynhMinhDang08022001\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDBASKETBALL\OneDrive\Máy tính\code_cong_ty\HuynhMinhDang08022001_dang\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8505" yWindow="3195" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="5640"/>
   </bookViews>
   <sheets>
     <sheet name="RFvalue_baseSW" sheetId="1" r:id="rId1"/>
     <sheet name="RFvalue_latestSW" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t>DID</t>
   </si>
@@ -31,7 +32,10 @@
     <t>Length (Byte)</t>
   </si>
   <si>
-    <t>Value</t>
+    <t>ASCII Value</t>
+  </si>
+  <si>
+    <t>HEX_Value</t>
   </si>
   <si>
     <t>BaseSW Name</t>
@@ -61,109 +65,115 @@
     <t>F194</t>
   </si>
   <si>
+    <t>Supplier Software number</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>S311 BL01_RC03</t>
+  </si>
+  <si>
+    <t>F189</t>
+  </si>
+  <si>
+    <t>ECUSoftwareVersionNumberDataIdentifier</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>SWC.6.0</t>
+  </si>
+  <si>
+    <t>F089</t>
+  </si>
+  <si>
+    <t>ECUHardwareVersionNumberDataIdentifier</t>
+  </si>
+  <si>
+    <t>HWC.2.0</t>
+  </si>
+  <si>
+    <t>F187</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>7917030-CD03</t>
+  </si>
+  <si>
+    <t>F188</t>
+  </si>
+  <si>
+    <t>Software Number</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>9212401-CD03</t>
+  </si>
+  <si>
+    <t>F170</t>
+  </si>
+  <si>
+    <t>FBL Version Information</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>V9.3</t>
+  </si>
+  <si>
+    <t>F1F4</t>
+  </si>
+  <si>
+    <t>vehicle configuration</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>F1F0</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>CA_S311_BL01_RC03</t>
+  </si>
+  <si>
+    <t>https://inside-docupedia.bosch.com/confluence/display/CNFV/CA_S311_BL01_RC03</t>
+  </si>
+  <si>
+    <t>F1F004</t>
+  </si>
+  <si>
+    <t>f1f0</t>
+  </si>
+  <si>
     <t>S311 BL01_RC05</t>
   </si>
   <si>
-    <t>F189</t>
-  </si>
-  <si>
-    <t>F089</t>
-  </si>
-  <si>
-    <t>F187</t>
-  </si>
-  <si>
-    <t>F188</t>
-  </si>
-  <si>
-    <t>F170</t>
-  </si>
-  <si>
-    <t>Supplier Software number</t>
-  </si>
-  <si>
-    <t>ECUSoftwareVersionNumberDataIdentifier</t>
-  </si>
-  <si>
-    <t>ECUHardwareVersionNumberDataIdentifier</t>
-  </si>
-  <si>
-    <t>Part Number</t>
-  </si>
-  <si>
-    <t>Software Number</t>
-  </si>
-  <si>
-    <t>FBL Version Information</t>
-  </si>
-  <si>
     <t>SWC.7.1</t>
   </si>
   <si>
-    <t>HWC.2.0</t>
-  </si>
-  <si>
-    <t>7917030-CD03</t>
-  </si>
-  <si>
-    <t>9212401-CD03</t>
-  </si>
-  <si>
-    <t>V9.3</t>
-  </si>
-  <si>
     <t>CA_S311_BL01_RC05</t>
   </si>
   <si>
-    <t>F1F4</t>
-  </si>
-  <si>
-    <t>F1F004</t>
-  </si>
-  <si>
-    <t>f1f0</t>
-  </si>
-  <si>
-    <t>CA_S311_BL01_RC03</t>
-  </si>
-  <si>
-    <t>https://inside-docupedia.bosch.com/confluence/display/CNFV/CA_S311_BL01_RC03</t>
-  </si>
-  <si>
-    <t>S311 BL01_RC03</t>
-  </si>
-  <si>
-    <t>SWC.6.0</t>
-  </si>
-  <si>
     <t>https://inside-docupedia.bosch.com/confluence/display/CNFV/CA_S311_BL01_RC05</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>vehicle configuration</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>F1F0</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -185,12 +195,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF172B4D"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -199,13 +203,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,12 +227,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0066CC"/>
         <bgColor rgb="FF0066CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -251,9 +256,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,14 +266,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -577,7 +581,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E11:E12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,9 +589,9 @@
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
     <col min="2" max="2" width="50" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.85546875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="30" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40" style="1" customWidth="1"/>
+    <col min="7" max="7" width="77.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
@@ -603,83 +607,85 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>35</v>
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>32</v>
+        <v>7</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
@@ -687,61 +693,62 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -750,7 +757,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,9 +765,9 @@
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
     <col min="2" max="2" width="50" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="1" customWidth="1"/>
+    <col min="4" max="5" width="30" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40" style="1" customWidth="1"/>
+    <col min="7" max="7" width="77.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
@@ -776,83 +783,85 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
@@ -860,41 +869,44 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -902,5 +914,6 @@
     <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>